<commit_message>
im either fixing shit or breaking it horribly
</commit_message>
<xml_diff>
--- a/data/sql/custom/db_world/Dialogue/Eversong Forest/RuinsOfSilvermoon.xlsx
+++ b/data/sql/custom/db_world/Dialogue/Eversong Forest/RuinsOfSilvermoon.xlsx
@@ -1,6 +1,23 @@
+
+<file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
+  <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+  <bookViews>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+  </bookViews>
+  <sheets>
+    <sheet name="FELENDREN" sheetId="1" r:id="rId1"/>
+    <sheet name="SOLANIAN" sheetId="2" r:id="rId2"/>
+    <sheet name="TZA'ZUHEN" sheetId="4" r:id="rId3"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId4"/>
+  </sheets>
+  <calcPr calcId="122211"/>
+</workbook>
+</file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="122">
   <si>
     <t>INRO_1</t>
   </si>
@@ -35,9 +52,6 @@
     <t>&lt;Attack&gt; I finished up my preparation, time to die...</t>
   </si>
   <si>
-    <t>DIALOGUE_1E</t>
-  </si>
-  <si>
     <t>conetx comment goes here</t>
   </si>
   <si>
@@ -57,9 +71,6 @@
   </si>
   <si>
     <t>Speak quickly or you'll be a skinned rat soon.</t>
-  </si>
-  <si>
-    <t>&lt;Attack&gt; Never mind, you're just another pathetic waste of Mana.</t>
   </si>
   <si>
     <t>While I do feel like I'm almost done, I have this odd urge to wait, to extend my Evocation and discharge further, and while I did and keep doing so, I find myself too bemused to worry, yet my thoughts feel empty.</t>
@@ -364,6 +375,15 @@
   </si>
   <si>
     <t>ORB_PONDER</t>
+  </si>
+  <si>
+    <t>&lt;Attack&gt; Never mind, you're just another pathetic drain on Mana.</t>
+  </si>
+  <si>
+    <t>DIALOGUE_a1A</t>
+  </si>
+  <si>
+    <t>DIALOGUE_a1B</t>
   </si>
 </sst>
 </file>
@@ -702,4 +722,641 @@
   <a:objectDefaults/>
   <a:extraClrSchemeLst/>
 </a:theme>
+</file>
+
+<file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C56"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="B23" sqref="B23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="20.7109375" customWidth="1"/>
+    <col min="2" max="2" width="112.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>120</v>
+      </c>
+      <c r="B5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>121</v>
+      </c>
+      <c r="B6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>94</v>
+      </c>
+      <c r="B9" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>98</v>
+      </c>
+      <c r="B10" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>96</v>
+      </c>
+      <c r="B11" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B12" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B13" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B14" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B15" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B16" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="17" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B17" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="18" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B18" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="19" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B19" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="20" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B20" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="21" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B21" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="22" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B22" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="23" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B23" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="24" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B24" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="25" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B25" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="26" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B26" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="27" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B27" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="28" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B28" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="29" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B29" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="30" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B30" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="31" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B31" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="32" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B32" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="33" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B33" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="34" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B34" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="35" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B35" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="36" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B36" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="37" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B37" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="38" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B38" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="39" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B39" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="40" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B40" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="41" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B41" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="42" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B42" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="43" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B43" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="44" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B44" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="45" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B45" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="46" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B46" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="47" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B47" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="48" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B48" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="49" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B49" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="50" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B50" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="51" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B51" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="52" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B52" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="53" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B53" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="54" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B54" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="55" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B55" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="56" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B56" t="s">
+        <v>84</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B18"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A19" sqref="A19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="20.85546875" customWidth="1"/>
+    <col min="2" max="2" width="82.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B2" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>37</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>38</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>39</v>
+      </c>
+      <c r="B5" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>40</v>
+      </c>
+      <c r="B6" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>42</v>
+      </c>
+      <c r="B7" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>43</v>
+      </c>
+      <c r="B8" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>44</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>45</v>
+      </c>
+      <c r="B10" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>46</v>
+      </c>
+      <c r="B11" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>47</v>
+      </c>
+      <c r="B12" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>108</v>
+      </c>
+      <c r="B13" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>110</v>
+      </c>
+      <c r="B14" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>112</v>
+      </c>
+      <c r="B15" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>116</v>
+      </c>
+      <c r="B16" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>117</v>
+      </c>
+      <c r="B17" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>118</v>
+      </c>
+      <c r="B18" t="s">
+        <v>115</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B14"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>90</v>
+      </c>
+      <c r="B1" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>91</v>
+      </c>
+      <c r="B2" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>44</v>
+      </c>
+      <c r="B7" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>94</v>
+      </c>
+      <c r="B8" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>98</v>
+      </c>
+      <c r="B9" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>96</v>
+      </c>
+      <c r="B10" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>101</v>
+      </c>
+      <c r="B11" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>45</v>
+      </c>
+      <c r="B12" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>104</v>
+      </c>
+      <c r="B13" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>103</v>
+      </c>
+      <c r="B14" t="s">
+        <v>100</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
before i fuck shit up
</commit_message>
<xml_diff>
--- a/data/sql/custom/db_world/Dialogue/Eversong Forest/RuinsOfSilvermoon.xlsx
+++ b/data/sql/custom/db_world/Dialogue/Eversong Forest/RuinsOfSilvermoon.xlsx
@@ -4,20 +4,21 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="2"/>
   </bookViews>
   <sheets>
-    <sheet name="FELENDREN" sheetId="1" r:id="rId1"/>
-    <sheet name="SOLANIAN" sheetId="2" r:id="rId2"/>
-    <sheet name="TZA'ZUHEN" sheetId="4" r:id="rId3"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId4"/>
+    <sheet name="MAGISTRIX_ERONA" sheetId="3" r:id="rId1"/>
+    <sheet name="RAELLIS" sheetId="5" r:id="rId2"/>
+    <sheet name="FELENDREN" sheetId="1" r:id="rId3"/>
+    <sheet name="SOLANIAN" sheetId="2" r:id="rId4"/>
+    <sheet name="TZA'ZUHEN" sheetId="4" r:id="rId5"/>
   </sheets>
   <calcPr calcId="122211"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="122">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="140">
   <si>
     <t>INRO_1</t>
   </si>
@@ -275,33 +276,12 @@
     <t>&lt;Return&gt; You're right, it's not worth the risk. What else?</t>
   </si>
   <si>
-    <t>A pup of withering Sin'dorei seed bravely walks into bloody chaff where it belongs, bravely knowing it's place as chow for the beasts. $b$bOr is the desire to release the beating necrotic nature in your soul so strong that you come to me with an uncanny request, dear child.</t>
-  </si>
-  <si>
-    <t>&lt;Attack&gt; I did not come here to listen to you rattle, bone-weaver.</t>
-  </si>
-  <si>
-    <t>Are you Tza'zuhen, the mongrel traitor-wizard whose mutt-skull I've come to split?</t>
-  </si>
-  <si>
-    <t>&lt;Attack&gt; Your feet I shall cut off, your innards cauterize, fingers I will nail together and then I'll hang you with hooks through your clavicles so all may look at you and know the Scourge will end.</t>
-  </si>
-  <si>
-    <t>Good speech Necromancer. You are the one responsible for splitting my beautiful Quel'Thalas in half I assume?</t>
-  </si>
-  <si>
     <t>INTRO_1A</t>
   </si>
   <si>
     <t>INTRO_1B</t>
   </si>
   <si>
-    <t>You dared come to me just to flee terrorized in your boots youngling. Now you bravely return. Admirable.</t>
-  </si>
-  <si>
-    <t>The name I was given for my eternal unlife is Tza'zuhen, Grand Osteomancer of Lordaeron. I was anointed by the spirit of Master Kel'Thuzad as I crafted his body into the masterwork your eternal Sunwell powered. $b$bIt is my duty now to bleed the blood-ears bone-dry so your permanent evaporation can please the Lord's dark desire.</t>
-  </si>
-  <si>
     <t>DIALOGUE_2A</t>
   </si>
   <si>
@@ -311,15 +291,9 @@
     <t>DIALOGUE_2C</t>
   </si>
   <si>
-    <t>I am here to command you to cease your aggression or face the wrath of Silvermoon now rather than later. These are our last and only terms. Accept them, or perish.</t>
-  </si>
-  <si>
     <t>DIALOGUE_2B</t>
   </si>
   <si>
-    <t>Grand Osteomancer, the grip of the Scourge in Quel'Thalas is weakening and reinforcements from three of four of Azeroth's great powers are coming. I request you make this easeir for both me and yourself and surrender, sparing me my people's lives and you the wrath of your tyrants.</t>
-  </si>
-  <si>
     <t>&lt;Attack&gt; That was mere formality, now we shall do battle as civilized folk.</t>
   </si>
   <si>
@@ -335,12 +309,6 @@
     <t>DIALOGUE_3A</t>
   </si>
   <si>
-    <t>What kindness you offer, elf. Why, I'd almost even forgotten my fealties over it.$b$bFear of death, that is something only the uninitiated have my kind friend, my only concern is when I will bring glory to my King.</t>
-  </si>
-  <si>
-    <t>&lt;Truce&gt; It is not a metter of when, your forces are being picked apart and your extermination will not succeed. If you pull back to spare the lives of our men and become someone else's problem, it would benefit both parties.</t>
-  </si>
-  <si>
     <t>&lt;Take Scroll of Scourge Magic&gt; Know thy enemy.</t>
   </si>
   <si>
@@ -380,10 +348,97 @@
     <t>&lt;Attack&gt; Never mind, you're just another pathetic drain on Mana.</t>
   </si>
   <si>
-    <t>DIALOGUE_a1A</t>
-  </si>
-  <si>
-    <t>DIALOGUE_a1B</t>
+    <t>A pup of withering Sin'dorei seed bravely walks into a pool of bloody chaff where it belongs, filled with bravery and crimson ecstasy it knows it's place as ritual chow for the beasts.$b$bOr perhaps you wish to sow and reap life-past-life so to zealously devour your fading bretheren, to release the beating necrotic nature already auditory pulsatining in the womb of your mind for... this not too uncommon request.$b$bSo why do you stand before me, enemy?</t>
+  </si>
+  <si>
+    <t>You dared come before me just to flee terrorized in your boots like the howling moon from dawn over the hill, youngling. Now you return, of stifled cauterized spirit defiant of the disquet that you hosted out of ignorance which mercifully let you live this far, even with endless wounds opening to the speeding maggots hiding in the wind eminating from mounds of melting, burning bodies that are no longer bodies.$b$bBrave as the sun which abandons all to darkest darkness every day yet always returning, always with the holiest certainty and greatest bravery, or at least until the master's hand reaches up to suffocate it with revelations of even it's own futility; so are you now here.$b$bFor what purpose is it?</t>
+  </si>
+  <si>
+    <t>&lt;Attack&gt; I did not come here to listen to you rattle, bone-weaver. Your delirious shrills will fade into a blind void where no sentient beasts that were before separated by oceans can be sewn together into alchemical horrors and save you from your penance.</t>
+  </si>
+  <si>
+    <t>&lt;Attack&gt; Your feet I shall cut off, your innards cauterize, fingers I will nail together and then I'll hang you with hooks through your clavicles so all may look at you and know the Scourge is ending.</t>
+  </si>
+  <si>
+    <t>The terrible name I was given by my master to take from into the grave and past, into the endless singularity of deaths and delirious truths, is Tza'zuhen, fermenter and sticher of the fluids of the skull, spine and heart with the coldest steel.$b$bI was anointed by the spirit of the then future Arch-Lich Kel'Thuzad as I crafted chains for his sacred chrysalis into the hand sculpted divine masterwork deserving of his eternal reward that your precious Sunwell powered.$b$bIt is now my duty to bleed the blood-ears bone-dry so your permanent evaporation into dry hot blight can please the Lord's dark desire.</t>
+  </si>
+  <si>
+    <t>I am here to command you to cease your aggression or face the wrath of Silvermoon now rather than later. These are our last and only terms. Accept them, or perish. Were this threat not well backed, I would not be standing in front of you, armed and stoic.</t>
+  </si>
+  <si>
+    <t>Kingpin of the Dead Scar, the grip of the Scourge in Quel'Thalas is weakening and reinforcements from three of four of Azeroth's great powers are coming sooner rather than later. I request you make this easeir for both me and yourself and surrender, sparing me my people's wounds, lives and grief, and you the wrath of your tyrants.</t>
+  </si>
+  <si>
+    <t>&lt;Truce&gt; It is not a metter of when, your forces are being picked apart and your unjust extermination will not succeed. If you pull back to spare the lives of our men, instead becoming someone else's problem, it would benefit both parties.</t>
+  </si>
+  <si>
+    <t>What warm kindness you offer to my sore head, relishable elf. Why, I'd almost even forgotten my covenant of fealties over this saccharine display from someone's last breath.$b$bFear of death, fear of secret monsters hiding in the blackness past one's burial, that is something only the uninitiated with instincts that are animalistic and minds that are vegetative have friend, my only concern is when I will bring glory to my King.</t>
+  </si>
+  <si>
+    <t>DIALOGUE_4A</t>
+  </si>
+  <si>
+    <t>DIALOGUE_4B</t>
+  </si>
+  <si>
+    <t>BUBBLE_5</t>
+  </si>
+  <si>
+    <t>&lt;Attack&gt; I've given you ample opportunity to surrender and retreat your bodies thinking your life and vitality might let you see some reason, yet you insult me by chatting. I can no longer risk you stalling nor escaping.</t>
+  </si>
+  <si>
+    <t>&lt;Choice, Truce&gt; Your armies are not forces of nature. If the Scourge could supply a truly infinite army it would have already conquered everything, and it wouldn't have struggled to hold as much of Quel'Thalas as it has. Instead we've risen like Pheonixes, the Plaguelands are cleansing, many are abandoning the Domination to join the Forsaken. If you wish to die and burn for your petty zeal, I cannot stop you and can only recommend you do not insult the intelligence of both your faction as well as my own.</t>
+  </si>
+  <si>
+    <t>&lt;The Necromancer pauses, seemingly both relaxed and frustrated as if trying to consciously get mad in the face of truth&gt;$b$bThe Scourge, we are not merely a pitiful army you dirty squirrel excrement ape. We are an infinite force of locusts that will devour the living and bring the truth of endless death to all.$b$bWhat makes you dare think I worry about losing donated bodies when your lives have to exert wee efforts to perservere into the future against passive inevitability itself?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Are you Tza'zuhen, the still-living mongrel traitor-wizard whose mutt-skull I've come to split? </t>
+  </si>
+  <si>
+    <t>Good speech, Necromancer. You are the one responsible for splitting my beautiful Quel'Thalas in half I assume? You don't seem to be undead.</t>
+  </si>
+  <si>
+    <t>BUBBLE_6</t>
+  </si>
+  <si>
+    <t>Does your speckless conscience speak reason? Or are you simply playing into my fears with your superior wit of strategy.</t>
+  </si>
+  <si>
+    <t>I shall retreat as to your advice, for now. Should you ever wish to taste the fruit of the Scourge, I will remember to vouch for you turning into more than a ghoul.</t>
+  </si>
+  <si>
+    <t>This was supposed to be a leisurely excursion in which I wore only a chrisom, but I wouldn't mind doing anything to assist before I leave.</t>
+  </si>
+  <si>
+    <t>It is always sad when pursuit of knowledge is cut short. I should consider solving this my thesis then.</t>
+  </si>
+  <si>
+    <t>Experiencing this incident to fawn over details of how the Sin'dorei perservere through uncommon circumstances in this cosmos interests me. Could you tell me about it?</t>
+  </si>
+  <si>
+    <t>&lt;Continue&gt;</t>
+  </si>
+  <si>
+    <t>I hope you enjoyed the last sleep of your jaunt in Sunstrider Isle, as it won't be able to host you anymore. The incident involving Felendren has gotten worse than initially estimated and has festered beyond any of our possessed remedies.</t>
+  </si>
+  <si>
+    <t>Malevolent destruction protrude from Falthrien Academy as a worm from a corpse of an animal slaughtered by a predator it could not understand. It is of origin too alien for our experts to ascertain correctly, tainting the Arcane and Fel aura of the isle with deathly fashion.$b$bThese rumbling qualities correlate with death and mingle as symbiosis of blossoms with bees, yet bearing synthesis that there is no well fashioned theorems on.$b$bThe destruction of the Sunwell by the Scourge sent adrift numerous disturbances that push us towards annihilation teetering on hideous oblivion, and this here unnatural event is no less cruel nor merciless.</t>
+  </si>
+  <si>
+    <t>If you wish to aid us in rebuilding our society from this hope-dispersing disaster and pull together what high hopes we had for Sunstrider Isle then you should learn how to deal with cunning combat.$b$bThe Burning Crystals forged from the knowledge hither brought from our bretheren in Outland were responsible for keeping the Mana Wyrms in Quel'Thalas tame. $b$bThey have been disturbed and made a target for culling. Like any intelligent creature, if they can fight in packs when threatened, they will, so I recommend you bring with you an ally to split the pressure.</t>
+  </si>
+  <si>
+    <t>Weapons, armour, gear you commonly find tends to be of relatively higher quality compared to the less common findings. However, it has no potential for improvement and has a limited lifecycle.</t>
+  </si>
+  <si>
+    <t>If you wish to aid us in the purging of this influence I recommend you arm and gear yourself in Thelyrn Sister's store, armor is especially valuable against smaller attacks in large quantities while for bigger attacks you're better off deflecting or dodging. And a good weapon will help you even if you prefer spells, as attacks are always useful for restoring mana.</t>
+  </si>
+  <si>
+    <t>DIALOGUE_4C</t>
+  </si>
+  <si>
+    <t>DIALOGUE_1E</t>
   </si>
 </sst>
 </file>
@@ -726,10 +781,132 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B12"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B1" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>44</v>
+      </c>
+      <c r="B5" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>87</v>
+      </c>
+      <c r="B6" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>45</v>
+      </c>
+      <c r="B7" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>95</v>
+      </c>
+      <c r="B8" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>46</v>
+      </c>
+      <c r="B9" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>138</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="O13" sqref="O13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1" t="s">
+        <v>136</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -775,7 +952,7 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>120</v>
+        <v>9</v>
       </c>
       <c r="B5" t="s">
         <v>6</v>
@@ -783,7 +960,7 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>121</v>
+        <v>139</v>
       </c>
       <c r="B6" t="s">
         <v>10</v>
@@ -807,7 +984,7 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>94</v>
+        <v>87</v>
       </c>
       <c r="B9" t="s">
         <v>16</v>
@@ -815,7 +992,7 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>98</v>
+        <v>90</v>
       </c>
       <c r="B10" t="s">
         <v>17</v>
@@ -823,10 +1000,10 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>96</v>
+        <v>89</v>
       </c>
       <c r="B11" t="s">
-        <v>119</v>
+        <v>108</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
@@ -1059,7 +1236,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B18"/>
   <sheetViews>
@@ -1171,50 +1348,50 @@
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>108</v>
+        <v>97</v>
       </c>
       <c r="B13" t="s">
-        <v>107</v>
+        <v>96</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>110</v>
+        <v>99</v>
       </c>
       <c r="B14" t="s">
-        <v>109</v>
+        <v>98</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>112</v>
+        <v>101</v>
       </c>
       <c r="B15" t="s">
-        <v>111</v>
+        <v>100</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>116</v>
+        <v>105</v>
       </c>
       <c r="B16" t="s">
-        <v>113</v>
+        <v>102</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>117</v>
+        <v>106</v>
       </c>
       <c r="B17" t="s">
-        <v>114</v>
+        <v>103</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>118</v>
+        <v>107</v>
       </c>
       <c r="B18" t="s">
-        <v>115</v>
+        <v>104</v>
       </c>
     </row>
   </sheetData>
@@ -1222,30 +1399,30 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B14"/>
+  <dimension ref="A1:B19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="B1" t="s">
-        <v>85</v>
+        <v>109</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="B2" t="s">
-        <v>92</v>
+        <v>110</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -1253,7 +1430,7 @@
         <v>4</v>
       </c>
       <c r="B3" t="s">
-        <v>89</v>
+        <v>125</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -1261,7 +1438,7 @@
         <v>5</v>
       </c>
       <c r="B4" t="s">
-        <v>87</v>
+        <v>124</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -1269,7 +1446,7 @@
         <v>7</v>
       </c>
       <c r="B5" t="s">
-        <v>86</v>
+        <v>111</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -1277,7 +1454,7 @@
         <v>9</v>
       </c>
       <c r="B6" t="s">
-        <v>88</v>
+        <v>112</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
@@ -1285,39 +1462,39 @@
         <v>44</v>
       </c>
       <c r="B7" t="s">
-        <v>93</v>
+        <v>113</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>94</v>
+        <v>87</v>
       </c>
       <c r="B8" t="s">
-        <v>97</v>
+        <v>114</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>98</v>
+        <v>90</v>
       </c>
       <c r="B9" t="s">
-        <v>99</v>
+        <v>115</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>96</v>
+        <v>89</v>
       </c>
       <c r="B10" t="s">
-        <v>102</v>
+        <v>93</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>101</v>
+        <v>92</v>
       </c>
       <c r="B11" t="s">
-        <v>95</v>
+        <v>88</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
@@ -1325,38 +1502,66 @@
         <v>45</v>
       </c>
       <c r="B12" t="s">
-        <v>105</v>
+        <v>117</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>104</v>
+        <v>95</v>
       </c>
       <c r="B13" t="s">
-        <v>106</v>
+        <v>116</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>103</v>
+        <v>94</v>
       </c>
       <c r="B14" t="s">
-        <v>100</v>
+        <v>91</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>46</v>
+      </c>
+      <c r="B15" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>118</v>
+      </c>
+      <c r="B16" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>119</v>
+      </c>
+      <c r="B17" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>120</v>
+      </c>
+      <c r="B18" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>126</v>
+      </c>
+      <c r="B19" t="s">
+        <v>128</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>